<commit_message>
remove banner action button for mobile
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylvester/spring-fest-2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCDDAD1-C90E-F548-94AF-160CEF35D1B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E35CE9F-0610-BB4F-AB89-D602D7296574}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{7E8D823B-DD30-FC4C-BBDC-CE3DD1ABEC48}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{7E8D823B-DD30-FC4C-BBDC-CE3DD1ABEC48}"/>
   </bookViews>
   <sheets>
     <sheet name="companies" sheetId="1" r:id="rId1"/>
@@ -1045,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4727805F-7934-0844-9796-E3018C4EFE86}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1339,13 +1339,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="E20" t="s">
         <v>162</v>
@@ -1353,13 +1353,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>125</v>
-      </c>
-      <c r="B21" t="s">
-        <v>84</v>
+        <v>164</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E21" t="s">
         <v>162</v>
@@ -1367,13 +1367,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>164</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>85</v>
+        <v>124</v>
+      </c>
+      <c r="B22" t="s">
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E22" t="s">
         <v>162</v>
@@ -1381,13 +1381,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>124</v>
-      </c>
-      <c r="B23" t="s">
-        <v>87</v>
+        <v>142</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>101</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E23" t="s">
         <v>162</v>
@@ -1395,13 +1395,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>142</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>101</v>
+        <v>123</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="E24" t="s">
         <v>162</v>
@@ -1416,7 +1416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21B1791-2BB9-1443-806D-06101E6A1429}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -2507,13 +2507,13 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{787313B1-31BB-304D-9955-2ED843BA0536}">
           <x14:formula1>
-            <xm:f>companies!$C$2:$C$20</xm:f>
+            <xm:f>companies!$C$2:$C$24</xm:f>
           </x14:formula1>
           <xm:sqref>B40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{56444AF4-0749-5145-9C64-1D8B9E6DA0C0}">
           <x14:formula1>
-            <xm:f>companies!$C$2:$C$24</xm:f>
+            <xm:f>companies!$C$2:$C$23</xm:f>
           </x14:formula1>
           <xm:sqref>A1:A1048576</xm:sqref>
         </x14:dataValidation>
@@ -2751,7 +2751,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{72720F4A-93BA-D744-8683-1AF250A9AEB6}">
           <x14:formula1>
-            <xm:f>companies!$A$2:$A$24</xm:f>
+            <xm:f>companies!$A$2:$A$23</xm:f>
           </x14:formula1>
           <xm:sqref>C1:C1048576</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
banner, header, sessions fix
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylvester/github-spring-fest-2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD4621E-F22B-5143-B9E2-2FF6B35714F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5CDAA1-5EB1-7D44-98B8-10FD1C2A9EAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39840" yWindow="4420" windowWidth="28800" windowHeight="17540" xr2:uid="{7E8D823B-DD30-FC4C-BBDC-CE3DD1ABEC48}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="5" xr2:uid="{7E8D823B-DD30-FC4C-BBDC-CE3DD1ABEC48}"/>
   </bookViews>
   <sheets>
     <sheet name="companies" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="195">
   <si>
     <t>NTT DATA</t>
   </si>
@@ -376,9 +376,6 @@
     <t>IT TRAINING SUPPLIER ～技術を育て、企業を育てる～</t>
   </si>
   <si>
-    <t>菊池真登</t>
-  </si>
-  <si>
     <t>懇親会</t>
   </si>
   <si>
@@ -462,9 +459,6 @@
   </si>
   <si>
     <t>LINEでは、企業･個店向けに公式アカウントというもの提供しています。公式アカウントでは多種多様な機能を提供しているのですが、その中の一つにチャット機能があります。そのチャットシステムにおける、Springの活用事例やアーキテクチャなどをご紹介致します。</t>
-  </si>
-  <si>
-    <t>長谷部良輔</t>
   </si>
   <si>
     <t>2013年 LINE入社。LINEの公式アカウントに関するサーバーサイドの開発を担当しています。以前はLINE Login, LINE Notify, LINE GAME Platformなどのサーバーサイド開発を担当していました</t>
@@ -605,6 +599,89 @@
 * 仕様の見える化とテストファーストによる品質保証
 * 自動テストと向き合った新卒の半年間
 など、SIerであるBTCにおけるハイアジリティを目指す取り組みの事例をご紹介いたします。</t>
+  </si>
+  <si>
+    <t>Spring Boot爆速開発超絶技巧</t>
+  </si>
+  <si>
+    <t>IntelliJ IDEAを使って開発する際、マウスやトラックパッドを使っていませんか？
+このセッションでは「なんとなく使っていても気づきにくい」、Spring
+Bootアプリケーションを開発する上で欠かせないキーボードショートカット、Dockerやデータベース連携、HTTPクライアント機能など、最新バージョンの魅力を余すことなくお伝えいたします。</t>
+  </si>
+  <si>
+    <t>サムライズムはIntelliJ
+IDEAで有名なJetBrainsやGitHubなど、開発に必要不可欠なツール群を取り扱っております。導入済みの方も、これから導入を検討されている方も、是非ブースにお立ち寄り頂き、最新情報を入手してください！</t>
+  </si>
+  <si>
+    <t xml:space="preserve">株式会社ビズリーチの取り組みとエンジニア組織
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">パンフレット等用いながら、ご来場者様へ研修サービスのご紹介をするほか、
+セッション聴講者の方から疑問点等あれば、回答させていただきます。
+</t>
+  </si>
+  <si>
+    <t>我々は日産が提供するコネクティドカーサービス「Nissan Connect」「Nissan Connect EV」を開発する部隊であり、サーバサイドをSpring Bootで開発しています。
+当ブースでは、上記アプリのご紹介や、開発プロセス等についてご紹介致します。
+IoTシステムの開発にご興味のある方・自動車好きの方・ソフトウェア内部に留まらない現実世界の「モノ」に繋がる開発に興味がある方は、是非ブースまでお越しください。我々は多くの仲間を求めています！</t>
+  </si>
+  <si>
+    <t>田中 竜介</t>
+  </si>
+  <si>
+    <t>長谷部 良輔</t>
+  </si>
+  <si>
+    <t>菊池 真登</t>
+  </si>
+  <si>
+    <t>楽天ペイ（オンライン決済）のアプリケーションエンジニアとして開発業務に携わっています。パブリッククラウドやコンテナオーケストラレーション、CI/CD などを良く触っています。</t>
+  </si>
+  <si>
+    <t>三宅 光太郎</t>
+  </si>
+  <si>
+    <t>専門はクラウドネイティブのミドルウェア開発および開発ツールの構築・導入</t>
+  </si>
+  <si>
+    <t>土屋 大樹</t>
+  </si>
+  <si>
+    <t>入社以来、テスト効率化・自動化に関する業務に従事。現在はコンテナ・k8sを活用したCI/CDパイプラインの設計・開発を行っている。</t>
+  </si>
+  <si>
+    <t>Spring Social でソーシャルログインを実装する</t>
+  </si>
+  <si>
+    <t>最近ソーシャルログインを提供するサービスは増えてきています。Spring Social は各SNS 専用のライブラリが用意されていて、これらを使ってソーシャルログインを実装することができます。
+このセッションでは、このソーシャルログイン機能を提供するWebアプリケーションを実装する方法を紹介します。</t>
+  </si>
+  <si>
+    <t>19, 20</t>
+  </si>
+  <si>
+    <t>　大規模エンタープライズシステム開発におけるSpringアプリケーションのDevOps適用事例</t>
+  </si>
+  <si>
+    <t>NRIでは社内の多くのプロジェクトでSpring Frameworkを利用したアプリケーションを開発しています。
+　本セッションではアプリケーション開発に欠かせないDevOpsに着目して、大規模プロジェクトでのコンテナ技術を活用したビルドやテストに関する事例を中心に、苦労した点や工夫した点をご紹介します。</t>
+  </si>
+  <si>
+    <t>aslead</t>
+  </si>
+  <si>
+    <t>DX時代のシステム開発およびオフィス業務の生産性向上のための製品・ソリューションの提供、技術サポートおよび導入支援・システム運用を提供する、asleadをご紹介します。</t>
+  </si>
+  <si>
+    <t>OpenStandia</t>
+  </si>
+  <si>
+    <t>オープンソースソフトウェア（OSS）を使用したシステムの構築や課題発生時の解決にあたり、OSSに関する技術サポート、導入支援、コンサルティングなどを提供するサービスです。Sprigをはじめ、様々なOSSのサポートを提供していますので、OSSでお困りの方は是非ブースまでお越しください。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日産コネクティドカーサービスの開発者募集！
+</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4727805F-7934-0844-9796-E3018C4EFE86}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1070,7 +1147,7 @@
         <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20">
@@ -1085,7 +1162,7 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="20">
@@ -1100,7 +1177,7 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="20">
@@ -1115,12 +1192,12 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
@@ -1130,12 +1207,12 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="20">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
@@ -1145,12 +1222,12 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="20">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>
@@ -1160,12 +1237,12 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="20">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s">
         <v>35</v>
@@ -1175,7 +1252,7 @@
       </c>
       <c r="D8" s="3"/>
       <c r="E8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="20">
@@ -1190,7 +1267,7 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="20">
@@ -1205,7 +1282,7 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="20">
@@ -1222,12 +1299,12 @@
         <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="20">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B12" t="s">
         <v>39</v>
@@ -1239,12 +1316,12 @@
         <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="20">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
         <v>40</v>
@@ -1254,7 +1331,7 @@
       </c>
       <c r="D13" s="3"/>
       <c r="E13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="20">
@@ -1269,12 +1346,12 @@
       </c>
       <c r="D14" s="3"/>
       <c r="E14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="20">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B15" t="s">
         <v>41</v>
@@ -1286,12 +1363,12 @@
         <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="20">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>
@@ -1301,12 +1378,12 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="20">
       <c r="A17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B17" t="s">
         <v>43</v>
@@ -1316,12 +1393,12 @@
       </c>
       <c r="D17" s="3"/>
       <c r="E17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="20">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B18" t="s">
         <v>45</v>
@@ -1331,12 +1408,12 @@
       </c>
       <c r="D18" s="3"/>
       <c r="E18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="20">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B19" t="s">
         <v>44</v>
@@ -1346,12 +1423,12 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B20" t="s">
         <v>84</v>
@@ -1360,12 +1437,12 @@
         <v>82</v>
       </c>
       <c r="E20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>85</v>
@@ -1374,12 +1451,12 @@
         <v>83</v>
       </c>
       <c r="E21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
         <v>87</v>
@@ -1388,12 +1465,12 @@
         <v>86</v>
       </c>
       <c r="E22" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>101</v>
@@ -1402,12 +1479,12 @@
         <v>88</v>
       </c>
       <c r="E23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B24" t="s">
         <v>77</v>
@@ -1416,7 +1493,7 @@
         <v>28</v>
       </c>
       <c r="E24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1428,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21B1791-2BB9-1443-806D-06101E6A1429}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1464,10 +1541,10 @@
         <v>56</v>
       </c>
       <c r="G1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1489,10 +1566,10 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1500,18 +1577,27 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17">
+    <row r="5" spans="1:8" ht="272">
       <c r="A5" s="5">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>189</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1519,18 +1605,27 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="306">
       <c r="A7" s="6">
         <v>4</v>
       </c>
+      <c r="B7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>186</v>
+      </c>
       <c r="D7" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+      <c r="E7">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="409.6">
@@ -1553,7 +1648,7 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1569,16 +1664,16 @@
         <v>102</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>78</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="10" customFormat="1">
@@ -1587,7 +1682,7 @@
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="10" customFormat="1" ht="409.6">
@@ -1595,10 +1690,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>133</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>134</v>
       </c>
       <c r="E13" s="10">
         <v>2</v>
@@ -1609,21 +1704,27 @@
         <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E14">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="323">
       <c r="A15" s="5">
         <v>10</v>
       </c>
+      <c r="B15" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>172</v>
+      </c>
       <c r="D15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E15">
         <v>3</v>
@@ -1656,10 +1757,10 @@
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>81</v>
@@ -1673,7 +1774,7 @@
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1681,10 +1782,10 @@
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1692,10 +1793,10 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E21">
         <v>14</v>
@@ -1720,7 +1821,7 @@
         <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1736,7 +1837,7 @@
         <v>20</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E25">
         <v>7</v>
@@ -1802,7 +1903,7 @@
         <v>104</v>
       </c>
       <c r="D32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1855,7 +1956,7 @@
         <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1866,7 +1967,7 @@
         <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1877,7 +1978,7 @@
         <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1888,7 +1989,7 @@
         <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1918,10 +2019,10 @@
         <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1929,10 +2030,10 @@
         <v>102</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1940,10 +2041,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1951,10 +2052,10 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1962,7 +2063,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
         <v>61</v>
@@ -1973,7 +2074,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C13" t="s">
         <v>63</v>
@@ -1984,10 +2085,10 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1995,10 +2096,10 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2006,7 +2107,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C16" t="s">
         <v>61</v>
@@ -2017,7 +2118,7 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C17" t="s">
         <v>63</v>
@@ -2028,10 +2129,10 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2039,10 +2140,10 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2050,7 +2151,7 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C20" t="s">
         <v>61</v>
@@ -2061,7 +2162,7 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21" t="s">
         <v>63</v>
@@ -2072,10 +2173,10 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2083,10 +2184,10 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2094,7 +2195,7 @@
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C24" t="s">
         <v>61</v>
@@ -2105,7 +2206,7 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C25" t="s">
         <v>63</v>
@@ -2116,10 +2217,10 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2127,7 +2228,7 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C27" t="s">
         <v>61</v>
@@ -2138,7 +2239,7 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C28" t="s">
         <v>63</v>
@@ -2149,10 +2250,10 @@
         <v>103</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2160,10 +2261,10 @@
         <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2171,7 +2272,7 @@
         <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C31" t="s">
         <v>61</v>
@@ -2182,7 +2283,7 @@
         <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
         <v>63</v>
@@ -2193,10 +2294,10 @@
         <v>104</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2242,7 +2343,7 @@
         <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2250,7 +2351,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2258,7 +2359,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2266,7 +2367,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2337,7 +2438,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2345,7 +2446,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2353,7 +2454,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2361,7 +2462,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2369,7 +2470,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2377,7 +2478,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2385,7 +2486,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2393,7 +2494,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2404,10 +2505,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9AA5683-37B4-5045-A1F9-BE9F8E8EF1D3}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView zoomScale="119" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2445,70 +2546,100 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="51">
       <c r="A4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C4" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="34">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="B5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="34">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="51">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="C7" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="102">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" ht="102">
+      <c r="A9" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+      <c r="B9" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="119">
+      <c r="A10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+      <c r="B10" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>22</v>
+      <c r="C11" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>135</v>
+      <c r="C15" s="14" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2521,7 +2652,7 @@
           <x14:formula1>
             <xm:f>companies!$C$2:$C$24</xm:f>
           </x14:formula1>
-          <xm:sqref>B40</xm:sqref>
+          <xm:sqref>B41</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{56444AF4-0749-5145-9C64-1D8B9E6DA0C0}">
           <x14:formula1>
@@ -2537,10 +2668,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326B0DA3-40C6-EF4E-A34F-32068C675173}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2581,13 +2712,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2598,7 +2729,7 @@
         <v>90</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -2621,7 +2752,7 @@
         <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D6" t="s">
         <v>79</v>
@@ -2680,10 +2811,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>179</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="68">
@@ -2694,7 +2825,7 @@
         <v>102</v>
       </c>
       <c r="C14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>103</v>
@@ -2705,13 +2836,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>178</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="85">
@@ -2719,13 +2850,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34">
@@ -2733,13 +2864,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="153">
@@ -2747,13 +2878,55 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>177</v>
+      </c>
+      <c r="C19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="34">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="51">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ios banner scroll fix
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylvester/github-spring-fest-2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B9F889-8E1F-E743-B0CA-BFB3C82EDE5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C566EB-238C-5248-A435-A77C93AAA79F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="1" xr2:uid="{7E8D823B-DD30-FC4C-BBDC-CE3DD1ABEC48}"/>
+    <workbookView xWindow="-38400" yWindow="-3580" windowWidth="38400" windowHeight="23540" activeTab="1" xr2:uid="{7E8D823B-DD30-FC4C-BBDC-CE3DD1ABEC48}"/>
   </bookViews>
   <sheets>
     <sheet name="companies" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="208">
   <si>
     <t>NTT DATA</t>
   </si>
@@ -563,10 +563,6 @@
 Bootアプリケーションを開発する上で欠かせないキーボードショートカット、Dockerやデータベース連携、HTTPクライアント機能など、最新バージョンの魅力を余すことなくお伝えいたします。</t>
   </si>
   <si>
-    <t>サムライズムはIntelliJ
-IDEAで有名なJetBrainsやGitHubなど、開発に必要不可欠なツール群を取り扱っております。導入済みの方も、これから導入を検討されている方も、是非ブースにお立ち寄り頂き、最新情報を入手してください！</t>
-  </si>
-  <si>
     <t xml:space="preserve">パンフレット等用いながら、ご来場者様へ研修サービスのご紹介をするほか、
 セッション聴講者の方から疑問点等あれば、回答させていただきます。
 </t>
@@ -617,9 +613,6 @@
   <si>
     <t xml:space="preserve">日産コネクティドカーサービスの開発者募集！
 </t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
   <si>
     <t>&lt;b&gt;&lt;a href="https://aslead.nri.co.jp" target="_blank"&gt;aslead&lt;/a&gt;&lt;/b&gt;
@@ -713,6 +706,22 @@
   </si>
   <si>
     <t>進藤さん</t>
+  </si>
+  <si>
+    <t>Springアプリケーションのテスト道具 使いどころ、使わないどころ</t>
+  </si>
+  <si>
+    <t>Springアプリケーションのテストにはたくさんの道具の選択肢があります。何を使えばいいか、いつ使うのが良いか、使い方はあっているか、使うべきでないとこらで使っていないか、、悩みは尽きません。
+本セッションではJUnitやSpringの機能、モック、Selenium、Dockerなどを使ったテストや、それらを使った際のありがちな問題、使うべきでない場面などをお話しします。</t>
+  </si>
+  <si>
+    <t>大阪在住のふつうのプログラマです。 Javaエンジニア養成読本でJava入門とかWEB+DB PRESSでJavaの新定石とか書きました。</t>
+  </si>
+  <si>
+    <t>サムライズムはIntelliJ</t>
+  </si>
+  <si>
+    <t>IDEAで有名なJetBrainsやGitHubなど、開発に必要不可欠なツール群を取り扱っております。導入済みの方も、これから導入を検討されている方も、是非ブースにお立ち寄り頂き、最新情報を入手してください！</t>
   </si>
 </sst>
 </file>
@@ -1532,8 +1541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21B1791-2BB9-1443-806D-06101E6A1429}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1574,7 +1583,7 @@
         <v>142</v>
       </c>
       <c r="I1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1615,14 +1624,14 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>178</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1638,10 +1647,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="E7">
         <v>18</v>
@@ -1666,7 +1675,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1675,6 +1684,9 @@
         <v>101</v>
       </c>
       <c r="D10" t="s">
+        <v>181</v>
+      </c>
+      <c r="F10" t="s">
         <v>9</v>
       </c>
       <c r="I10" t="s">
@@ -1691,6 +1703,9 @@
       <c r="C11" s="10" t="s">
         <v>144</v>
       </c>
+      <c r="D11" t="s">
+        <v>181</v>
+      </c>
       <c r="E11" s="9" t="s">
         <v>148</v>
       </c>
@@ -1704,7 +1719,7 @@
       </c>
       <c r="C12" s="10"/>
       <c r="E12" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>118</v>
@@ -1782,7 +1797,7 @@
         <v>140</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>51</v>
@@ -1877,7 +1892,7 @@
         <v>8</v>
       </c>
       <c r="F26" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1891,12 +1906,18 @@
         <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="340">
       <c r="A28" s="5">
         <v>23</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="E28">
         <v>10</v>
@@ -1913,7 +1934,7 @@
         <v>11</v>
       </c>
       <c r="F29" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1927,7 +1948,7 @@
         <v>23</v>
       </c>
       <c r="F30" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1941,7 +1962,7 @@
         <v>24</v>
       </c>
       <c r="F31" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2551,7 +2572,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2588,29 +2609,29 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="51">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="34">
       <c r="A4" t="s">
         <v>27</v>
       </c>
+      <c r="B4" t="s">
+        <v>206</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="119">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>180</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="51">
@@ -2618,7 +2639,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2642,19 +2663,20 @@
         <v>84</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>182</v>
-      </c>
+      <c r="B10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
@@ -2674,9 +2696,6 @@
     <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>82</v>
-      </c>
-      <c r="B14" t="s">
-        <v>180</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>130</v>
@@ -2710,8 +2729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326B0DA3-40C6-EF4E-A34F-32068C675173}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2747,7 +2766,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2761,7 +2780,7 @@
         <v>119</v>
       </c>
       <c r="D3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="68">
@@ -2775,7 +2794,7 @@
         <v>135</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2789,7 +2808,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2845,6 +2864,9 @@
       <c r="B11" t="s">
         <v>92</v>
       </c>
+      <c r="D11" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
@@ -2859,13 +2881,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C13" t="s">
         <v>133</v>
       </c>
       <c r="D13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="68">
@@ -2887,13 +2909,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="85">
@@ -2943,13 +2965,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C19" t="s">
         <v>115</v>
       </c>
       <c r="D19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="34">
@@ -2957,13 +2979,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="51">
@@ -2971,13 +2993,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="68">
@@ -2985,13 +3007,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C22" t="s">
         <v>118</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="34">
@@ -2999,13 +3021,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C23" t="s">
         <v>118</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="18">
@@ -3013,7 +3035,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="18">
@@ -3021,7 +3043,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed console tagbangers link
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylvester/github-spring-fest-2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F579031-3F37-F445-8112-B1C834401900}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBC32A2-8DF9-964D-8FBF-53E9C3BF510A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="6" xr2:uid="{7E8D823B-DD30-FC4C-BBDC-CE3DD1ABEC48}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="5" xr2:uid="{7E8D823B-DD30-FC4C-BBDC-CE3DD1ABEC48}"/>
   </bookViews>
   <sheets>
     <sheet name="companies" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="257">
   <si>
     <t>NTT DATA</t>
   </si>
@@ -925,6 +925,9 @@
   </si>
   <si>
     <t>Acroquest Technology株式会社所属。Spring Bootを使ったWebアプリ開発がメイン。最近はGoで開発することも多い。</t>
+  </si>
+  <si>
+    <t>DX 時代を想定したアーキテクチャ、開発プロセスについて、豆蔵の現場のアーキテクトやコンサルタントがご相談に乗ります。ブースにて豆蔵グッズも配布しますので、是非お越し下さい</t>
   </si>
 </sst>
 </file>
@@ -2977,8 +2980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9AA5683-37B4-5045-A1F9-BE9F8E8EF1D3}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView zoomScale="91" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3090,9 +3093,12 @@
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" ht="51">
       <c r="A11" t="s">
         <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="68">
@@ -3139,7 +3145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326B0DA3-40C6-EF4E-A34F-32068C675173}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="115" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
PR-05 Modify Session & Booth
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="companies" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="263">
   <si>
     <t>NTT DATA</t>
   </si>
@@ -674,9 +674,6 @@
     <t xml:space="preserve">テクニカルセールス本部
 Associate Principal Solution Architect
 </t>
-  </si>
-  <si>
-    <t>ストレスレスな Spring Boot を使った Web アプリケーション開発環境。Jib, Skaffold, Google Kubernetes Engine, Docker, Cloud Code などの紹介。</t>
   </si>
   <si>
     <t>Spring Developer のための コンテナ入門</t>
@@ -899,9 +896,6 @@
     <t>寺田 佳央</t>
   </si>
   <si>
-    <t>基調講演</t>
-  </si>
-  <si>
     <t>Spring Boot アプリの運用が楽になる？ Pivotal と Microsoft が共同開発した専用 PaaS「Azure Spring Cloud」のご紹介 !!</t>
   </si>
   <si>
@@ -949,6 +943,20 @@
 * 仕様の見える化とテストファーストによる品質保証
 * 自動テストと向き合った新卒の半年間
 など、SIerであるBTCにおけるハイアジリティを目指す取り組みの事例をご紹介いたします。</t>
+  </si>
+  <si>
+    <t>基調講演：From Spring Boot 2.2 to Spring Boot 2.3</t>
+  </si>
+  <si>
+    <t>ストレスレスな Spring Boot を使った Web アプリケーション開発環境の紹介</t>
+  </si>
+  <si>
+    <t>Google Kubernetes Engine（GKE）は、コンテナ化されたアプリケーションをデプロイするための、本番環境に対応したマネージド型環境です。最新のテクノロジーを利用して、デベロッパーの生産性、リソースの効率性、自動運用、オープンソースの柔軟性の向上を図り、製品化までの時間を短縮します。
+2015 年にリリースされた Kubernetes Engine は、12 年以上にわたって Gmail や YouTube などのサービスをコンテナ内で実行してきた Google の豊富な経験に基づいて構築されています。Kubernetes Engine を使用すると、独自の Kubernetes クラスタをインストールして管理、操作する必要がなくなり、Kubernetes の設定から稼働までを短時間で完了できます。
+こちらのブースでは、Google Kubernetes Engine（GKE）, Docker, Cloud Code, Jib, Skaffold などを紹介します。</t>
+  </si>
+  <si>
+    <t>4,6</t>
   </si>
 </sst>
 </file>
@@ -1782,8 +1790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1840,7 +1848,10 @@
         <v>0.2</v>
       </c>
       <c r="B3" t="s">
-        <v>251</v>
+        <v>259</v>
+      </c>
+      <c r="E3" t="s">
+        <v>262</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" t="s">
@@ -1855,10 +1866,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E4">
         <v>34</v>
@@ -1872,7 +1883,7 @@
         <v>140</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -1883,10 +1894,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>169</v>
@@ -1900,7 +1911,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>185</v>
@@ -1992,16 +2003,16 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" t="s">
         <v>220</v>
-      </c>
-      <c r="C12" t="s">
-        <v>221</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>169</v>
       </c>
       <c r="E12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F12"/>
       <c r="G12"/>
@@ -2016,7 +2027,7 @@
         <v>83</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D13"/>
       <c r="E13">
@@ -2046,10 +2057,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15">
@@ -2061,10 +2072,10 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E16">
         <v>28</v>
@@ -2075,10 +2086,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="E17">
         <v>27</v>
@@ -2109,10 +2120,10 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
+        <v>207</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>209</v>
       </c>
       <c r="E19">
         <v>7</v>
@@ -2124,10 +2135,10 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E20">
         <v>6</v>
@@ -2152,10 +2163,10 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
+        <v>232</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>169</v>
@@ -2169,10 +2180,10 @@
         <v>18</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="E23">
         <v>32</v>
@@ -2186,7 +2197,7 @@
         <v>149</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E24">
         <v>18</v>
@@ -2197,10 +2208,10 @@
         <v>20</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="E25">
         <v>4</v>
@@ -2228,7 +2239,7 @@
         <v>137</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E27">
         <v>17</v>
@@ -2280,10 +2291,10 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
+        <v>200</v>
+      </c>
+      <c r="C30" t="s">
         <v>201</v>
-      </c>
-      <c r="C30" t="s">
-        <v>202</v>
       </c>
       <c r="E30">
         <v>29</v>
@@ -2319,7 +2330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -2339,7 +2350,7 @@
         <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D1" t="s">
         <v>70</v>
@@ -2434,7 +2445,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -2448,7 +2459,7 @@
         <v>4.2</v>
       </c>
       <c r="B9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -2462,7 +2473,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -2932,7 +2943,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2940,7 +2951,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3010,7 +3021,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView zoomScale="91" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3058,10 +3069,10 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="160" x14ac:dyDescent="0.2">
@@ -3069,7 +3080,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="64" x14ac:dyDescent="0.2">
@@ -3083,12 +3094,15 @@
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
+      <c r="B7" t="s">
+        <v>260</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>194</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="96" x14ac:dyDescent="0.2">
@@ -3127,7 +3141,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="64" x14ac:dyDescent="0.2">
@@ -3135,7 +3149,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -3233,7 +3247,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>117</v>
@@ -3275,13 +3289,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3289,10 +3303,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8" t="s">
         <v>210</v>
-      </c>
-      <c r="D8" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3300,10 +3314,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3311,10 +3325,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" t="s">
         <v>218</v>
-      </c>
-      <c r="D10" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3333,10 +3347,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>230</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3506,10 +3520,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -3545,13 +3559,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -3559,13 +3573,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -3573,13 +3587,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C30" t="s">
         <v>100</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -3587,10 +3601,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -3598,10 +3612,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -3609,13 +3623,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C33" t="s">
         <v>134</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="176" x14ac:dyDescent="0.2">
@@ -3623,13 +3637,13 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C34" t="s">
         <v>105</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PR-06 Modify Session place
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="19960" windowHeight="20540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="companies" sheetId="1" r:id="rId1"/>
@@ -464,10 +464,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">受託開発におけるハイアジリティへのとりくみ
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">寺島 秀樹
 </t>
   </si>
@@ -958,12 +954,16 @@
   <si>
     <t>4,6</t>
   </si>
+  <si>
+    <t xml:space="preserve">受託開発でテストファーストしたらXXXを早期発見できてハイアジリティになったはなし
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1036,6 +1036,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1057,7 +1063,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1091,6 +1097,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1790,15 +1797,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="73.33203125" customWidth="1"/>
-    <col min="3" max="3" width="159" customWidth="1"/>
+    <col min="3" max="3" width="130.5" customWidth="1"/>
     <col min="4" max="4" width="23.5" customWidth="1"/>
     <col min="5" max="5" width="26.1640625" customWidth="1"/>
     <col min="6" max="6" width="105.33203125" customWidth="1"/>
@@ -1832,7 +1839,7 @@
         <v>124</v>
       </c>
       <c r="I1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1848,10 +1855,10 @@
         <v>0.2</v>
       </c>
       <c r="B3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" t="s">
@@ -1861,15 +1868,15 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="E4">
         <v>34</v>
@@ -1880,10 +1887,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -1894,45 +1901,45 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>216</v>
-      </c>
       <c r="D6" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E6">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="128" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>4.0999999999999996</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>129</v>
@@ -1944,18 +1951,18 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>4.2</v>
       </c>
       <c r="B9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="D9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E9">
         <v>25</v>
@@ -1965,15 +1972,15 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>5</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -2003,23 +2010,23 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C12" t="s">
         <v>219</v>
       </c>
-      <c r="C12" t="s">
-        <v>220</v>
-      </c>
       <c r="D12" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F12"/>
       <c r="G12"/>
       <c r="H12"/>
       <c r="I12"/>
     </row>
-    <row r="13" spans="1:9" s="9" customFormat="1" ht="216" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" s="9" customFormat="1" ht="198" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>8</v>
       </c>
@@ -2027,7 +2034,7 @@
         <v>83</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D13"/>
       <c r="E13">
@@ -2057,10 +2064,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>241</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15">
@@ -2072,31 +2079,31 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
+        <v>253</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>255</v>
       </c>
       <c r="E16">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="192" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="176" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="E17">
         <v>27</v>
       </c>
       <c r="F17" s="13"/>
     </row>
-    <row r="18" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>13</v>
       </c>
@@ -2104,7 +2111,7 @@
         <v>112</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9">
@@ -2120,126 +2127,126 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>208</v>
       </c>
       <c r="E19">
         <v>7</v>
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E20">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="E21">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>17</v>
       </c>
       <c r="B22" t="s">
+        <v>231</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>233</v>
-      </c>
       <c r="D22" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E22">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>18</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>239</v>
       </c>
       <c r="E23">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E24">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>20</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="E25">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>21</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E26">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="128" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>22</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>137</v>
+        <v>262</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E27">
         <v>17</v>
@@ -2250,14 +2257,14 @@
         <v>23</v>
       </c>
       <c r="B28" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>175</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>176</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>103</v>
@@ -2274,10 +2281,10 @@
         <v>122</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E29">
         <v>5</v>
@@ -2291,10 +2298,10 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
+        <v>199</v>
+      </c>
+      <c r="C30" t="s">
         <v>200</v>
-      </c>
-      <c r="C30" t="s">
-        <v>201</v>
       </c>
       <c r="E30">
         <v>29</v>
@@ -2330,8 +2337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2350,9 +2357,9 @@
         <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2366,8 +2373,8 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>110</v>
+      <c r="D2" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2380,7 +2387,7 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="17" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2394,8 +2401,8 @@
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>111</v>
+      <c r="D4" s="17" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2408,8 +2415,8 @@
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
-        <v>110</v>
+      <c r="D5" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2422,7 +2429,7 @@
       <c r="C6">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="17" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2436,7 +2443,7 @@
       <c r="C7">
         <v>3</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="17" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2445,12 +2452,12 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="17" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2459,12 +2466,12 @@
         <v>4.2</v>
       </c>
       <c r="B9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="17" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2473,12 +2480,12 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="17" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2492,7 +2499,7 @@
       <c r="C11">
         <v>6</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="17" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2506,7 +2513,7 @@
       <c r="C12">
         <v>6</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="17" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2520,7 +2527,7 @@
       <c r="C13">
         <v>6</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="17" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2534,7 +2541,7 @@
       <c r="C14">
         <v>7</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="17" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2548,7 +2555,7 @@
       <c r="C15">
         <v>7</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="17" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2562,7 +2569,7 @@
       <c r="C16">
         <v>7</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="17" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2576,7 +2583,7 @@
       <c r="C17">
         <v>8</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="17" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2590,7 +2597,7 @@
       <c r="C18">
         <v>8</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="17" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2604,7 +2611,7 @@
       <c r="C19">
         <v>8</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="17" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2618,8 +2625,8 @@
       <c r="C20">
         <v>9</v>
       </c>
-      <c r="D20" t="s">
-        <v>111</v>
+      <c r="D20" s="17" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2632,8 +2639,8 @@
       <c r="C21">
         <v>9</v>
       </c>
-      <c r="D21" t="s">
-        <v>110</v>
+      <c r="D21" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2646,7 +2653,7 @@
       <c r="C22">
         <v>9</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="17" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2660,7 +2667,7 @@
       <c r="C23">
         <v>9</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="17" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2674,7 +2681,7 @@
       <c r="C24">
         <v>10</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="17" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2688,7 +2695,7 @@
       <c r="C25">
         <v>10</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="17" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2702,7 +2709,7 @@
       <c r="C26">
         <v>10</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="17" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2716,7 +2723,7 @@
       <c r="C27">
         <v>10</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="17" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2730,8 +2737,8 @@
       <c r="C28">
         <v>11</v>
       </c>
-      <c r="D28" t="s">
-        <v>111</v>
+      <c r="D28" s="17" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -2744,8 +2751,8 @@
       <c r="C29">
         <v>11</v>
       </c>
-      <c r="D29" t="s">
-        <v>110</v>
+      <c r="D29" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -2758,7 +2765,7 @@
       <c r="C30">
         <v>11</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="17" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2772,7 +2779,7 @@
       <c r="C31">
         <v>11</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="17" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2786,8 +2793,8 @@
       <c r="C32">
         <v>12</v>
       </c>
-      <c r="D32" t="s">
-        <v>110</v>
+      <c r="D32" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2943,7 +2950,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2951,7 +2958,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3058,10 +3065,10 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -3069,10 +3076,10 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="160" x14ac:dyDescent="0.2">
@@ -3080,7 +3087,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="64" x14ac:dyDescent="0.2">
@@ -3088,10 +3095,10 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="112" x14ac:dyDescent="0.2">
@@ -3099,10 +3106,10 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="96" x14ac:dyDescent="0.2">
@@ -3121,10 +3128,10 @@
         <v>81</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -3132,7 +3139,7 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -3141,7 +3148,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="64" x14ac:dyDescent="0.2">
@@ -3149,7 +3156,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -3219,13 +3226,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3239,7 +3246,7 @@
         <v>104</v>
       </c>
       <c r="D3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -3247,13 +3254,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>117</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3261,13 +3268,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3289,13 +3296,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3303,10 +3310,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D8" t="s">
         <v>209</v>
-      </c>
-      <c r="D8" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3314,10 +3321,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3325,10 +3332,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>216</v>
+      </c>
+      <c r="D10" t="s">
         <v>217</v>
-      </c>
-      <c r="D10" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3339,7 +3346,7 @@
         <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -3347,10 +3354,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3358,13 +3365,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C13" t="s">
         <v>115</v>
       </c>
       <c r="D13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -3386,13 +3393,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -3428,13 +3435,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C18" t="s">
         <v>102</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -3442,13 +3449,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
         <v>101</v>
       </c>
       <c r="D19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -3456,13 +3463,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -3470,13 +3477,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -3484,13 +3491,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C22" t="s">
         <v>103</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -3498,13 +3505,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C23" t="s">
         <v>103</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -3512,7 +3519,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -3520,10 +3527,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -3531,13 +3538,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C26" t="s">
         <v>119</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -3545,13 +3552,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C27" t="s">
         <v>107</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -3559,13 +3566,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -3573,13 +3580,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -3587,13 +3594,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C30" t="s">
         <v>100</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="96" x14ac:dyDescent="0.2">
@@ -3601,10 +3608,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="112" x14ac:dyDescent="0.2">
@@ -3612,10 +3619,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -3623,13 +3630,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C33" t="s">
         <v>134</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="176" x14ac:dyDescent="0.2">
@@ -3637,13 +3644,13 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C34" t="s">
         <v>105</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>